<commit_message>
Added meeting protocol of meeting with Gerd Holweg
</commit_message>
<xml_diff>
--- a/doc/Featurelist_v01-0.xlsx
+++ b/doc/Featurelist_v01-0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\1_Semester\ITP-1\MultiPlay\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -491,10 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,6 +847,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>